<commit_message>
switched high score to 90 with 91 as special case, made genotypes global, added glCalc function
</commit_message>
<xml_diff>
--- a/data/referee-performance-celegans.xlsx
+++ b/data/referee-performance-celegans.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bin\referee\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregg/bin/referee/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718EA7AA-8D45-3342-B551-3CBE5F8E0AD1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="48" windowWidth="28620" windowHeight="12912"/>
+    <workbookView xWindow="120" yWindow="460" windowWidth="28620" windowHeight="12920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="c.elegans-info" sheetId="4" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="43">
   <si>
     <t>Num procs</t>
   </si>
@@ -148,12 +149,15 @@
   </si>
   <si>
     <t>Avg. base quality of all sites</t>
+  </si>
+  <si>
+    <t>WITH GL CALCS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -278,6 +282,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -313,6 +334,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -488,19 +526,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="56.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -508,7 +546,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -516,7 +554,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -524,7 +562,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -535,7 +573,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -543,7 +581,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -551,7 +589,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -559,7 +597,7 @@
         <v>99265117</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -567,7 +605,7 @@
         <v>96250753</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -575,7 +613,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -583,7 +621,7 @@
         <v>8168</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -591,7 +629,7 @@
         <v>92891231</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -599,7 +637,7 @@
         <v>3907</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -607,7 +645,7 @@
         <v>31.45</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -615,7 +653,7 @@
         <v>16.920000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -623,7 +661,7 @@
         <v>5.0196625459600002</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -631,7 +669,7 @@
         <v>90.834476003899994</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -639,7 +677,7 @@
         <v>4.9394561258399996</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>41</v>
       </c>
@@ -647,7 +685,7 @@
         <v>58.537063336099997</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -655,7 +693,7 @@
         <v>56.778786187000001</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -669,24 +707,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -706,7 +744,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -726,7 +764,7 @@
         <v>162.546875</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -746,7 +784,7 @@
         <v>162.546875</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -766,7 +804,7 @@
         <v>166.8984375</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -786,7 +824,7 @@
         <v>166.8984375</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -806,7 +844,7 @@
         <v>170.0859375</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -826,7 +864,7 @@
         <v>162.515625</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -846,7 +884,7 @@
         <v>162.515625</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -866,7 +904,7 @@
         <v>162.515625</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -886,7 +924,7 @@
         <v>698.7578125</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -906,7 +944,7 @@
         <v>698.7421875</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -926,7 +964,7 @@
         <v>698.7421875</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -946,7 +984,7 @@
         <v>698.7421875</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -966,7 +1004,7 @@
         <v>702.87890625</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3</v>
       </c>
@@ -986,7 +1024,7 @@
         <v>162.515625</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
@@ -1006,7 +1044,7 @@
         <v>162.515625</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -1026,7 +1064,7 @@
         <v>162.515625</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1046,7 +1084,7 @@
         <v>863.859375</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -1066,7 +1104,7 @@
         <v>863.859375</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -1086,7 +1124,7 @@
         <v>863.859375</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -1106,7 +1144,7 @@
         <v>863.859375</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1126,7 +1164,7 @@
         <v>863.859375</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -1146,7 +1184,12 @@
         <v>867.99609375</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>4</v>
       </c>
@@ -1166,7 +1209,7 @@
         <v>162.515625</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>4</v>
       </c>
@@ -1186,7 +1229,7 @@
         <v>162.515625</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>4</v>
       </c>
@@ -1206,7 +1249,7 @@
         <v>162.515625</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>4</v>
       </c>
@@ -1226,7 +1269,7 @@
         <v>1037.8984375</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4</v>
       </c>
@@ -1246,7 +1289,7 @@
         <v>1029.38671875</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>4</v>
       </c>
@@ -1266,7 +1309,7 @@
         <v>1029.35546875</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4</v>
       </c>
@@ -1286,7 +1329,7 @@
         <v>1029.35546875</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>4</v>
       </c>
@@ -1306,7 +1349,7 @@
         <v>1029.35546875</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>4</v>
       </c>
@@ -1326,7 +1369,7 @@
         <v>1029.35546875</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>4</v>
       </c>
@@ -1346,7 +1389,7 @@
         <v>1033.5</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>5</v>
       </c>
@@ -1366,7 +1409,7 @@
         <v>162.515625</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>5</v>
       </c>
@@ -1386,7 +1429,7 @@
         <v>162.515625</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>5</v>
       </c>
@@ -1406,7 +1449,7 @@
         <v>162.515625</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>5</v>
       </c>
@@ -1426,7 +1469,7 @@
         <v>1196.14453125</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>5</v>
       </c>
@@ -1446,7 +1489,7 @@
         <v>1196.14453125</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>5</v>
       </c>
@@ -1466,7 +1509,7 @@
         <v>1196.14453125</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>5</v>
       </c>
@@ -1486,7 +1529,7 @@
         <v>1196.14453125</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>5</v>
       </c>
@@ -1506,7 +1549,7 @@
         <v>1196.14453125</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>5</v>
       </c>
@@ -1526,7 +1569,7 @@
         <v>1196.14453125</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>5</v>
       </c>
@@ -1546,7 +1589,7 @@
         <v>1196.14453125</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>5</v>
       </c>
@@ -1573,24 +1616,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1610,7 +1653,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1630,7 +1673,7 @@
         <v>162.4453125</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1650,7 +1693,7 @@
         <v>257.2734375</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1670,7 +1713,7 @@
         <v>257.2734375</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1690,7 +1733,7 @@
         <v>257.2734375</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1710,7 +1753,7 @@
         <v>257.2734375</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1730,7 +1773,7 @@
         <v>162.4453125</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1750,7 +1793,7 @@
         <v>257.33203125</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1770,7 +1813,7 @@
         <v>257.33203125</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1790,7 +1833,7 @@
         <v>1176.6484375</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -1810,7 +1853,7 @@
         <v>1176.6171875</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1830,7 +1873,7 @@
         <v>1176.6171875</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1850,7 +1893,7 @@
         <v>1176.6171875</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1870,7 +1913,7 @@
         <v>1176.6171875</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1890,7 +1933,7 @@
         <v>162.4453125</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
@@ -1910,7 +1953,7 @@
         <v>257.33203125</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -1930,7 +1973,7 @@
         <v>257.33203125</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1950,7 +1993,7 @@
         <v>1531.890625</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -1970,7 +2013,7 @@
         <v>1531.875</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -1990,7 +2033,7 @@
         <v>1531.859375</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2010,7 +2053,7 @@
         <v>1531.859375</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2030,7 +2073,7 @@
         <v>1531.859375</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2050,7 +2093,7 @@
         <v>1531.859375</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>4</v>
       </c>
@@ -2070,7 +2113,7 @@
         <v>162.4453125</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>4</v>
       </c>
@@ -2090,7 +2133,7 @@
         <v>257.33203125</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>4</v>
       </c>
@@ -2110,7 +2153,7 @@
         <v>257.33203125</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>4</v>
       </c>
@@ -2130,7 +2173,7 @@
         <v>1887.125</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4</v>
       </c>
@@ -2150,7 +2193,7 @@
         <v>1887.125</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>4</v>
       </c>
@@ -2170,7 +2213,7 @@
         <v>1887.109375</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4</v>
       </c>
@@ -2190,7 +2233,7 @@
         <v>1887.09375</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>4</v>
       </c>
@@ -2210,7 +2253,7 @@
         <v>1887.09375</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2230,7 +2273,7 @@
         <v>1887.09375</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>4</v>
       </c>
@@ -2250,7 +2293,7 @@
         <v>1887.09375</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>5</v>
       </c>
@@ -2270,7 +2313,7 @@
         <v>162.4453125</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>5</v>
       </c>
@@ -2290,7 +2333,7 @@
         <v>257.33203125</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>5</v>
       </c>
@@ -2310,7 +2353,7 @@
         <v>257.33203125</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>5</v>
       </c>
@@ -2330,7 +2373,7 @@
         <v>2242.3515625</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>5</v>
       </c>
@@ -2350,7 +2393,7 @@
         <v>2242.3515625</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>5</v>
       </c>
@@ -2370,7 +2413,7 @@
         <v>2242.3515625</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>5</v>
       </c>
@@ -2390,7 +2433,7 @@
         <v>2242.3359375</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>5</v>
       </c>
@@ -2410,7 +2453,7 @@
         <v>2242.3359375</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>5</v>
       </c>
@@ -2430,7 +2473,7 @@
         <v>2242.3359375</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>5</v>
       </c>
@@ -2450,7 +2493,7 @@
         <v>2242.3359375</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>5</v>
       </c>
@@ -2476,24 +2519,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2513,7 +2556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2533,7 +2576,7 @@
         <v>162.4453125</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2553,7 +2596,7 @@
         <v>262.09375</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2573,7 +2616,7 @@
         <v>262.2265625</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2593,7 +2636,7 @@
         <v>262.2265625</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2613,7 +2656,7 @@
         <v>262.2265625</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -2633,7 +2676,7 @@
         <v>162.4453125</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2653,7 +2696,7 @@
         <v>261.9765625</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2673,7 +2716,7 @@
         <v>261.9765625</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2693,7 +2736,7 @@
         <v>1185.3046875</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2713,7 +2756,7 @@
         <v>1185.3046875</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2733,7 +2776,7 @@
         <v>1185.3046875</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2753,7 +2796,7 @@
         <v>1185.3046875</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2773,7 +2816,7 @@
         <v>1185.3046875</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3</v>
       </c>
@@ -2793,7 +2836,7 @@
         <v>162.4453125</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
@@ -2813,7 +2856,7 @@
         <v>261.9765625</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -2833,7 +2876,7 @@
         <v>261.9765625</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2853,7 +2896,7 @@
         <v>1545.875</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -2873,7 +2916,7 @@
         <v>1545.84375</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2893,7 +2936,7 @@
         <v>1545.84375</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2913,7 +2956,7 @@
         <v>1545.84375</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2933,7 +2976,7 @@
         <v>1545.84375</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2953,7 +2996,7 @@
         <v>1545.84375</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>4</v>
       </c>
@@ -2973,7 +3016,7 @@
         <v>162.4453125</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>4</v>
       </c>
@@ -2993,7 +3036,7 @@
         <v>261.9765625</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>4</v>
       </c>
@@ -3013,7 +3056,7 @@
         <v>261.9765625</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>4</v>
       </c>
@@ -3033,7 +3076,7 @@
         <v>1906.421875</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4</v>
       </c>
@@ -3053,7 +3096,7 @@
         <v>1906.421875</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>4</v>
       </c>
@@ -3073,7 +3116,7 @@
         <v>1906.390625</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4</v>
       </c>
@@ -3093,7 +3136,7 @@
         <v>1906.390625</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>4</v>
       </c>
@@ -3113,7 +3156,7 @@
         <v>1906.390625</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>4</v>
       </c>
@@ -3133,7 +3176,7 @@
         <v>1906.390625</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>4</v>
       </c>
@@ -3153,7 +3196,7 @@
         <v>1906.390625</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>5</v>
       </c>
@@ -3173,7 +3216,7 @@
         <v>162.4453125</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>5</v>
       </c>
@@ -3193,7 +3236,7 @@
         <v>261.9765625</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>5</v>
       </c>
@@ -3213,7 +3256,7 @@
         <v>261.9765625</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>5</v>
       </c>
@@ -3233,7 +3276,7 @@
         <v>2266.98046875</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>5</v>
       </c>
@@ -3253,7 +3296,7 @@
         <v>2266.93359375</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>5</v>
       </c>
@@ -3273,7 +3316,7 @@
         <v>2266.93359375</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>5</v>
       </c>
@@ -3293,7 +3336,7 @@
         <v>2266.93359375</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>5</v>
       </c>
@@ -3313,7 +3356,7 @@
         <v>2266.93359375</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>5</v>
       </c>
@@ -3333,7 +3376,7 @@
         <v>2266.93359375</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>5</v>
       </c>
@@ -3353,7 +3396,7 @@
         <v>2266.93359375</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
read scaff and pos right away in refCalc rather than after file type is assigned
</commit_message>
<xml_diff>
--- a/data/referee-performance-celegans.xlsx
+++ b/data/referee-performance-celegans.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregg/bin/referee/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718EA7AA-8D45-3342-B551-3CBE5F8E0AD1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E2A1B3-4096-F04C-B98E-90E70EFE1227}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="28620" windowHeight="12920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="100" yWindow="460" windowWidth="28620" windowHeight="12920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="c.elegans-info" sheetId="4" r:id="rId1"/>

</xml_diff>